<commit_message>
all backend apis are done
</commit_message>
<xml_diff>
--- a/docs/api.xlsx
+++ b/docs/api.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$I$39</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="171">
   <si>
     <t>done</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>发送cookie，发送基本信息查询请求，得到满足要求的用户个人信息</t>
+  </si>
+  <si>
+    <t>user(用户)</t>
   </si>
   <si>
     <t>用户行程信息查询</t>
@@ -699,7 +702,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,12 +711,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -905,12 +902,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1034,10 +1040,10 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1046,16 +1052,16 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1067,70 +1073,73 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1142,54 +1151,54 @@
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1198,68 +1207,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1326,21 +1344,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1612,19 +1630,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="$A30:$XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.7" customWidth="1"/>
-    <col min="2" max="2" width="20.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9" style="5"/>
-    <col min="4" max="4" width="21.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.1" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9" style="6"/>
+    <col min="4" max="4" width="21.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="23.1" style="7" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="55.25" customWidth="1"/>
     <col min="8" max="8" width="54.625" customWidth="1"/>
@@ -1632,1060 +1650,1117 @@
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1" spans="1:9">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="2:9">
-      <c r="B10" s="13" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:9">
+      <c r="A10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="2:9">
-      <c r="B11" s="13" t="s">
+    <row r="11" s="1" customFormat="1" spans="1:9">
+      <c r="A11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" spans="1:9">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="17" t="s">
+    <row r="12" s="1" customFormat="1" spans="1:9">
+      <c r="A12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="17" t="s">
+    <row r="13" s="1" customFormat="1" spans="1:9">
+      <c r="A13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" ht="16" customHeight="1" spans="1:9">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="17" t="s">
+    <row r="14" s="2" customFormat="1" ht="16" customHeight="1" spans="1:9">
+      <c r="A14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" spans="1:9">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="17" t="s">
+    <row r="15" s="1" customFormat="1" spans="1:9">
+      <c r="A15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" spans="1:9">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="17" t="s">
+    <row r="16" s="1" customFormat="1" spans="1:9">
+      <c r="A16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" s="2" customFormat="1" spans="1:9">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="17" t="s">
+    <row r="18" s="1" customFormat="1" spans="1:9">
+      <c r="A18" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20" t="s">
+      <c r="H18" s="17"/>
+      <c r="I18" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" ht="16" customHeight="1" spans="1:9">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="17" t="s">
+    <row r="19" s="1" customFormat="1" ht="16" customHeight="1" spans="1:9">
+      <c r="A19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="H19" s="17"/>
+      <c r="I19" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" spans="1:9">
-      <c r="A20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="17" t="s">
+    <row r="20" s="1" customFormat="1" spans="1:9">
+      <c r="A20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12" t="s">
+      <c r="H21" s="12"/>
+      <c r="I21" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" s="4" customFormat="1" spans="1:9">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="17" t="s">
+    <row r="22" s="3" customFormat="1" spans="1:9">
+      <c r="A22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="H22" s="18"/>
+      <c r="I22" s="18" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11" t="s">
+      <c r="H23" s="12"/>
+      <c r="I23" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" spans="1:9">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="17" t="s">
+    <row r="24" s="1" customFormat="1" spans="1:9">
+      <c r="A24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="21" t="s">
+      <c r="H24" s="17"/>
+      <c r="I24" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" spans="1:9">
-      <c r="A25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="17" t="s">
+    <row r="25" s="1" customFormat="1" spans="1:9">
+      <c r="A25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20" t="s">
+      <c r="H25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="2:9">
-      <c r="B26" s="13" t="s">
+    <row r="26" s="1" customFormat="1" spans="1:9">
+      <c r="A26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="16" t="s">
+      <c r="H26" s="17"/>
+      <c r="I26" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="1" spans="2:9">
-      <c r="B27" s="13" t="s">
+    <row r="27" s="1" customFormat="1" spans="1:9">
+      <c r="A27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16" t="s">
+      <c r="H27" s="17"/>
+      <c r="I27" s="18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:9">
-      <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="28" s="1" customFormat="1" spans="1:9">
+      <c r="A28" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:9">
-      <c r="A29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="17" t="s">
+    <row r="29" s="1" customFormat="1" spans="1:9">
+      <c r="A29" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="21" t="s">
+      <c r="I29" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" spans="1:9">
-      <c r="A30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="17" t="s">
+    <row r="30" s="1" customFormat="1" spans="1:9">
+      <c r="A30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:9">
+      <c r="A31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D31" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E31" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="G30" s="21" t="s">
+      <c r="F31" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H31" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="I30" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" s="2" customFormat="1" spans="1:9">
-      <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="17" t="s">
+      <c r="I31" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="1" spans="1:9">
+      <c r="A32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D32" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F31" s="21" t="s">
+      <c r="E32" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="F32" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="I31" s="20" t="s">
+      <c r="H32" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" s="2" customFormat="1" spans="1:9">
-      <c r="A32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="17" t="s">
+      <c r="I32" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" s="1" customFormat="1" spans="1:9">
+      <c r="A33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D33" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E33" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="G32" s="21" t="s">
+      <c r="F33" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H33" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="I32" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" s="2" customFormat="1" spans="1:9">
-      <c r="A33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="17" t="s">
+      <c r="I33" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" spans="1:9">
+      <c r="A34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F33" s="20" t="s">
+      <c r="E34" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="F34" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="I33" s="20" t="s">
+      <c r="H34" s="18" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="34" s="2" customFormat="1" spans="1:9">
-      <c r="A34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="I34" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" spans="1:9">
+      <c r="A35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C35" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D35" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21" t="s">
+      <c r="F35" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="I34" s="20" t="s">
+      <c r="G35" s="18"/>
+      <c r="H35" s="18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="35" s="2" customFormat="1" spans="1:9">
-      <c r="A35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="17" t="s">
+      <c r="I35" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" s="1" customFormat="1" spans="1:9">
+      <c r="A36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D36" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="F35" s="21" t="s">
+      <c r="E36" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="F36" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="G36" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="H36" s="18" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="36" s="2" customFormat="1" ht="34.5" customHeight="1" spans="1:9">
-      <c r="A36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="17" t="s">
+      <c r="I36" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="1" ht="34.5" customHeight="1" spans="1:9">
+      <c r="A37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C37" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D37" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F36" s="20" t="s">
+      <c r="E37" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="F37" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="G37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="H37" s="24" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="37" s="1" customFormat="1" spans="2:9">
-      <c r="B37" s="13" t="s">
+      <c r="I37" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="1" spans="1:9">
+      <c r="A38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C38" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D38" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="15" t="s">
+      <c r="E38" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="F38" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="G38" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="I37" s="16" t="s">
+      <c r="H38" s="18" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="38" ht="36" customHeight="1" spans="8:9">
-      <c r="H38" s="27" t="s">
+      <c r="I38" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="I38" s="7" t="s">
+    </row>
+    <row r="39" s="5" customFormat="1" ht="36" customHeight="1" spans="1:9">
+      <c r="A39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="29" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="39" ht="31.5" customHeight="1" spans="7:8">
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="7:7">
-      <c r="G40" s="7" t="s">
+      <c r="I39" s="31" t="s">
         <v>165</v>
       </c>
     </row>
+    <row r="40" ht="31.5" customHeight="1" spans="7:8">
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+    </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="30" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="30" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="30" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="30" t="s">
         <v>169</v>
       </c>
     </row>
+    <row r="45" spans="7:7">
+      <c r="G45" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:I38">
+  <autoFilter ref="B1:I39">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C$1:C$1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"POST"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>"GET"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C29 C31:C1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"GET"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>